<commit_message>
adding provenance to metabolism examples
</commit_message>
<xml_diff>
--- a/examples/kinetic_metabolic_model/data.xlsx
+++ b/examples/kinetic_metabolic_model/data.xlsx
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6867" uniqueCount="3083">
   <si>
-    <t>!!!ObjTables objTablesVersion='1.0.1' date='2020-06-03 15:21:24'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-06-03 15:21:24' objTablesVersion='1.0.1'</t>
+    <t>!!!ObjTables objTablesVersion='1.0.9' date='2020-06-03 15:21:24' comment='Data obtained from Khodayari &amp; Maranas, Nature Communications, 2016, DOI: 10.1038/ncomms13806'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-06-03 15:21:24' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Id</t>
@@ -57,7 +57,7 @@
     <t>periplasm</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-06-03 15:21:24' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-06-03 15:21:24' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Formula</t>
@@ -2496,7 +2496,7 @@
     <t>D-Xylulose 5-phosphate</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-06-03 15:21:24' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-06-03 15:21:24' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Id (iAF1260 [Ref1])</t>
@@ -9829,7 +9829,7 @@
 7.0	2,4-diaminobutyrate	Escherichia coli		485898	2D-image
 15.0	glycine	Escherichia coli		485898	2D-image
 13.0	L-alanine	Escherichia coli		485898	2D-image
-110.0	L-asparagine	Escherichia coli		485898 	2D-image
+110.0	L-asparagine	Escherichia coli		485898	2D-image
 14.0	L-isoleucine	Escherichia coli		485898	2D-image
 5.5	L-leucine	Escherichia coli		485898	2D-image
 40.0	L-methionine	Escherichia coli		485898	2D-image
@@ -12122,7 +12122,7 @@
     <t>&lt;wc_utils.workbook.core.Formula object at 0x7f055c2166d0&gt;</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-06-03 15:21:24' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-06-03 15:21:24' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Title</t>
@@ -12182,7 +12182,7 @@
     <t>Keseler IM, Mackie A, Peralta-Gil M, Santos-Zavaleta A, Gama-Castro S, Bonavides-Martínez C, Fulcher C, Huerta AM, Kothari A, Krummenacker M, Latendresse M, Muñiz-Rascado L, Ong Q, Paley S, Schröder I, Shearer AG, Subhraveti P, Travers M, Weerasinghe D, Weiss V, Collado-Vides J, Gunsalus RP, Paulsen I, Karp PD.</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-06-03 15:21:24' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-06-03 15:21:24' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Reaction</t>
@@ -12200,10 +12200,10 @@
     <t>competitive inhibition</t>
   </si>
   <si>
+    <t>activation</t>
+  </si>
+  <si>
     <t>mixed inhibition</t>
-  </si>
-  <si>
-    <t>activation</t>
   </si>
 </sst>
 </file>
@@ -12267,7 +12267,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -38790,10 +38790,10 @@
     </row>
     <row r="3" spans="1:4" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>2030</v>
+        <v>2219</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>197</v>
+        <v>597</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -38804,10 +38804,10 @@
     </row>
     <row r="4" spans="1:4" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>897</v>
+        <v>2554</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>597</v>
+        <v>536</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -38818,38 +38818,38 @@
     </row>
     <row r="5" spans="1:4" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>2092</v>
+        <v>2110</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>597</v>
+        <v>536</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>2092</v>
+        <v>2110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>594</v>
+        <v>720</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>2554</v>
+        <v>2228</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>594</v>
+        <v>720</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
@@ -38860,10 +38860,10 @@
     </row>
     <row r="8" spans="1:4" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>2554</v>
+        <v>2228</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>720</v>
+        <v>792</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
@@ -38874,10 +38874,10 @@
     </row>
     <row r="9" spans="1:4" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>2749</v>
+        <v>1319</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>720</v>
+        <v>792</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -38888,10 +38888,10 @@
     </row>
     <row r="10" spans="1:4" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>2219</v>
+        <v>1319</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>720</v>
+        <v>570</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -38902,10 +38902,10 @@
     </row>
     <row r="11" spans="1:4" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>2219</v>
+        <v>2617</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>536</v>
+        <v>570</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -38916,24 +38916,24 @@
     </row>
     <row r="12" spans="1:4" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>1319</v>
+        <v>2617</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>536</v>
+        <v>247</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>1319</v>
+        <v>2587</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>567</v>
+        <v>247</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -38944,10 +38944,10 @@
     </row>
     <row r="14" spans="1:4" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>2228</v>
+        <v>2587</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>567</v>
+        <v>365</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -38958,10 +38958,10 @@
     </row>
     <row r="15" spans="1:4" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>2228</v>
+        <v>2335</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>691</v>
+        <v>365</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
@@ -38972,10 +38972,10 @@
     </row>
     <row r="16" spans="1:4" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>1329</v>
+        <v>2335</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>691</v>
+        <v>597</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -38986,10 +38986,10 @@
     </row>
     <row r="17" spans="1:4" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>1329</v>
+        <v>2529</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>570</v>
+        <v>597</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -39000,10 +39000,10 @@
     </row>
     <row r="18" spans="1:4" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>2110</v>
+        <v>2529</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>570</v>
+        <v>594</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>
@@ -39014,10 +39014,10 @@
     </row>
     <row r="19" spans="1:4" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>2110</v>
+        <v>2335</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>4</v>
@@ -39028,10 +39028,10 @@
     </row>
     <row r="20" spans="1:4" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>2110</v>
+        <v>1976</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>280</v>
+        <v>594</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>4</v>
@@ -39042,66 +39042,66 @@
     </row>
     <row r="21" spans="1:4" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>1916</v>
+        <v>1976</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>280</v>
+        <v>600</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>3081</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.01" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>1916</v>
+        <v>2110</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>646</v>
+        <v>600</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.01" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>2259</v>
+        <v>2092</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>646</v>
+        <v>600</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>3081</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.01" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>2259</v>
+        <v>2092</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>473</v>
+        <v>280</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.01" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>2259</v>
+        <v>2065</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>608</v>
+        <v>280</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>4</v>
@@ -39112,10 +39112,10 @@
     </row>
     <row r="26" spans="1:4" ht="15.01" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>1930</v>
+        <v>2065</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>608</v>
+        <v>685</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>4</v>
@@ -39126,66 +39126,66 @@
     </row>
     <row r="27" spans="1:4" ht="15.01" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>1930</v>
+        <v>2529</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>326</v>
+        <v>685</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.01" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>2092</v>
+        <v>2722</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>326</v>
+        <v>280</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.01" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>2378</v>
+        <v>2722</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>326</v>
+        <v>709</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.01" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>2607</v>
+        <v>2754</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>326</v>
+        <v>280</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.01" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>2767</v>
+        <v>2754</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>326</v>
+        <v>646</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>4</v>
@@ -39196,66 +39196,66 @@
     </row>
     <row r="32" spans="1:4" ht="15.01" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>2767</v>
+        <v>2731</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>743</v>
+        <v>646</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.01" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>2773</v>
+        <v>2731</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>743</v>
+        <v>172</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.01" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>2773</v>
+        <v>2731</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>326</v>
+        <v>697</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.01" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>2451</v>
+        <v>2754</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>326</v>
+        <v>697</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.01" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>2451</v>
+        <v>2717</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>247</v>
+        <v>697</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>4</v>
@@ -39266,10 +39266,10 @@
     </row>
     <row r="37" spans="1:4" ht="15.01" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>1078</v>
+        <v>2717</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>247</v>
+        <v>559</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>4</v>
@@ -39280,10 +39280,10 @@
     </row>
     <row r="38" spans="1:4" ht="15.01" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>1078</v>
+        <v>2015</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>268</v>
+        <v>559</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>4</v>
@@ -39294,24 +39294,24 @@
     </row>
     <row r="39" spans="1:4" ht="15.01" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>1007</v>
+        <v>2015</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>268</v>
+        <v>720</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.01" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>1559</v>
+        <v>2110</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>268</v>
+        <v>697</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>4</v>
@@ -39322,10 +39322,10 @@
     </row>
     <row r="41" spans="1:4" ht="15.01" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>1559</v>
+        <v>2959</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>661</v>
+        <v>697</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>4</v>
@@ -39336,10 +39336,10 @@
     </row>
     <row r="42" spans="1:4" ht="15.01" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>1567</v>
+        <v>2959</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>661</v>
+        <v>326</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>4</v>
@@ -39350,10 +39350,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.01" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>1078</v>
+        <v>2110</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>4</v>
@@ -39364,24 +39364,24 @@
     </row>
     <row r="44" spans="1:4" ht="15.01" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>2430</v>
+        <v>2219</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.01" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>2430</v>
+        <v>2219</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>247</v>
+        <v>792</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>4</v>
@@ -39392,10 +39392,10 @@
     </row>
     <row r="46" spans="1:4" ht="15.01" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>2451</v>
+        <v>2219</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>4</v>
@@ -39406,24 +39406,24 @@
     </row>
     <row r="47" spans="1:4" ht="15.01" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>1028</v>
+        <v>2587</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.01" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>1028</v>
+        <v>2110</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>259</v>
+        <v>368</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>4</v>
@@ -39434,10 +39434,10 @@
     </row>
     <row r="49" spans="1:4" ht="15.01" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>1028</v>
+        <v>2123</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>4</v>
@@ -39448,10 +39448,10 @@
     </row>
     <row r="50" spans="1:4" ht="15.01" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>1028</v>
+        <v>2123</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>4</v>
@@ -39462,10 +39462,10 @@
     </row>
     <row r="51" spans="1:4" ht="15.01" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>1019</v>
+        <v>1282</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>4</v>
@@ -39476,10 +39476,10 @@
     </row>
     <row r="52" spans="1:4" ht="15.01" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>1019</v>
+        <v>1477</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>4</v>
@@ -39490,10 +39490,10 @@
     </row>
     <row r="53" spans="1:4" ht="15.01" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>1159</v>
+        <v>1477</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>312</v>
+        <v>470</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>4</v>
@@ -39504,24 +39504,24 @@
     </row>
     <row r="54" spans="1:4" ht="15.01" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>1159</v>
+        <v>2092</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>640</v>
+        <v>470</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.01" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>1111</v>
+        <v>2699</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>640</v>
+        <v>470</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>4</v>
@@ -39532,10 +39532,10 @@
     </row>
     <row r="56" spans="1:4" ht="15.01" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>2506</v>
+        <v>2110</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>640</v>
+        <v>470</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>4</v>
@@ -39546,10 +39546,10 @@
     </row>
     <row r="57" spans="1:4" ht="15.01" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>2506</v>
+        <v>1319</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>4</v>
@@ -39560,10 +39560,10 @@
     </row>
     <row r="58" spans="1:4" ht="15.01" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>2110</v>
+        <v>1477</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>476</v>
+        <v>567</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>4</v>
@@ -39574,10 +39574,10 @@
     </row>
     <row r="59" spans="1:4" ht="15.01" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>2825</v>
+        <v>1259</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>476</v>
+        <v>567</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>4</v>
@@ -39588,10 +39588,10 @@
     </row>
     <row r="60" spans="1:4" ht="15.01" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>2825</v>
+        <v>1259</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>326</v>
+        <v>286</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>4</v>
@@ -39602,10 +39602,10 @@
     </row>
     <row r="61" spans="1:4" ht="15.01" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>2825</v>
+        <v>2506</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>301</v>
+        <v>567</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>4</v>
@@ -39616,10 +39616,10 @@
     </row>
     <row r="62" spans="1:4" ht="15.01" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>2110</v>
+        <v>2506</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>301</v>
+        <v>720</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>4</v>
@@ -39633,7 +39633,7 @@
         <v>2506</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>301</v>
+        <v>818</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>4</v>
@@ -39644,10 +39644,10 @@
     </row>
     <row r="64" spans="1:4" ht="15.01" customHeight="1">
       <c r="A64" s="3" t="s">
-        <v>2554</v>
+        <v>2228</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>301</v>
+        <v>818</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>4</v>
@@ -39658,10 +39658,10 @@
     </row>
     <row r="65" spans="1:4" ht="15.01" customHeight="1">
       <c r="A65" s="3" t="s">
-        <v>2839</v>
+        <v>2506</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>301</v>
+        <v>550</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>4</v>
@@ -39672,10 +39672,10 @@
     </row>
     <row r="66" spans="1:4" ht="15.01" customHeight="1">
       <c r="A66" s="3" t="s">
-        <v>2839</v>
+        <v>2228</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>4</v>
@@ -39686,10 +39686,10 @@
     </row>
     <row r="67" spans="1:4" ht="15.01" customHeight="1">
       <c r="A67" s="3" t="s">
-        <v>1373</v>
+        <v>2506</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>527</v>
+        <v>658</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>4</v>
@@ -39700,10 +39700,10 @@
     </row>
     <row r="68" spans="1:4" ht="15.01" customHeight="1">
       <c r="A68" s="3" t="s">
-        <v>1373</v>
+        <v>2923</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>326</v>
+        <v>658</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>4</v>
@@ -39714,10 +39714,10 @@
     </row>
     <row r="69" spans="1:4" ht="15.01" customHeight="1">
       <c r="A69" s="3" t="s">
-        <v>1373</v>
+        <v>2672</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>306</v>
+        <v>658</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>4</v>
@@ -39728,10 +39728,10 @@
     </row>
     <row r="70" spans="1:4" ht="15.01" customHeight="1">
       <c r="A70" s="3" t="s">
-        <v>1129</v>
+        <v>2672</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>4</v>
@@ -39742,35 +39742,35 @@
     </row>
     <row r="71" spans="1:4" ht="15.01" customHeight="1">
       <c r="A71" s="3" t="s">
-        <v>2084</v>
+        <v>1916</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>306</v>
+        <v>658</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.01" customHeight="1">
       <c r="A72" s="3" t="s">
-        <v>2084</v>
+        <v>1916</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>326</v>
+        <v>441</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.01" customHeight="1">
       <c r="A73" s="3" t="s">
-        <v>2092</v>
+        <v>1916</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>306</v>
@@ -39784,7 +39784,7 @@
     </row>
     <row r="74" spans="1:4" ht="15.01" customHeight="1">
       <c r="A74" s="3" t="s">
-        <v>2101</v>
+        <v>2790</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>306</v>
@@ -39793,15 +39793,15 @@
         <v>4</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.01" customHeight="1">
       <c r="A75" s="3" t="s">
-        <v>2101</v>
+        <v>992</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>4</v>
@@ -39812,24 +39812,24 @@
     </row>
     <row r="76" spans="1:4" ht="15.01" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>2110</v>
+        <v>992</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>306</v>
+        <v>591</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.01" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>1305</v>
+        <v>2959</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>306</v>
+        <v>591</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>4</v>
@@ -39840,24 +39840,24 @@
     </row>
     <row r="78" spans="1:4" ht="15.01" customHeight="1">
       <c r="A78" s="3" t="s">
-        <v>1305</v>
+        <v>2092</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.01" customHeight="1">
       <c r="A79" s="3" t="s">
-        <v>2473</v>
+        <v>1926</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>603</v>
+        <v>306</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>4</v>
@@ -39868,52 +39868,52 @@
     </row>
     <row r="80" spans="1:4" ht="15.01" customHeight="1">
       <c r="A80" s="3" t="s">
-        <v>1305</v>
+        <v>1926</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>321</v>
+        <v>646</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.01" customHeight="1">
       <c r="A81" s="3" t="s">
-        <v>2451</v>
+        <v>1926</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>321</v>
+        <v>658</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.01" customHeight="1">
       <c r="A82" s="3" t="s">
-        <v>1289</v>
+        <v>1926</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>321</v>
+        <v>280</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.01" customHeight="1">
       <c r="A83" s="3" t="s">
-        <v>1289</v>
+        <v>2055</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>4</v>
@@ -39924,10 +39924,10 @@
     </row>
     <row r="84" spans="1:4" ht="15.01" customHeight="1">
       <c r="A84" s="3" t="s">
-        <v>1298</v>
+        <v>2055</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>318</v>
+        <v>476</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>4</v>
@@ -39938,10 +39938,10 @@
     </row>
     <row r="85" spans="1:4" ht="15.01" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>1298</v>
+        <v>2554</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>461</v>
+        <v>476</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>4</v>
@@ -39952,10 +39952,10 @@
     </row>
     <row r="86" spans="1:4" ht="15.01" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>2110</v>
+        <v>2554</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>318</v>
+        <v>792</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>4</v>
@@ -39966,10 +39966,10 @@
     </row>
     <row r="87" spans="1:4" ht="15.01" customHeight="1">
       <c r="A87" s="3" t="s">
-        <v>2506</v>
+        <v>2554</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>4</v>
@@ -39980,10 +39980,10 @@
     </row>
     <row r="88" spans="1:4" ht="15.01" customHeight="1">
       <c r="A88" s="3" t="s">
-        <v>2110</v>
+        <v>1436</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>4</v>
@@ -39994,10 +39994,10 @@
     </row>
     <row r="89" spans="1:4" ht="15.01" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>2617</v>
+        <v>1436</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>321</v>
+        <v>803</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>4</v>
@@ -40008,10 +40008,10 @@
     </row>
     <row r="90" spans="1:4" ht="15.01" customHeight="1">
       <c r="A90" s="3" t="s">
-        <v>2617</v>
+        <v>2055</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>434</v>
+        <v>803</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>4</v>
@@ -40022,10 +40022,10 @@
     </row>
     <row r="91" spans="1:4" ht="15.01" customHeight="1">
       <c r="A91" s="3" t="s">
-        <v>1149</v>
+        <v>1245</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>434</v>
+        <v>803</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>4</v>
@@ -40036,10 +40036,10 @@
     </row>
     <row r="92" spans="1:4" ht="15.01" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>1149</v>
+        <v>1237</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>740</v>
+        <v>803</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>4</v>
@@ -40050,10 +40050,10 @@
     </row>
     <row r="93" spans="1:4" ht="15.01" customHeight="1">
       <c r="A93" s="3" t="s">
-        <v>1530</v>
+        <v>1436</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>740</v>
+        <v>579</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>4</v>
@@ -40064,10 +40064,10 @@
     </row>
     <row r="94" spans="1:4" ht="15.01" customHeight="1">
       <c r="A94" s="3" t="s">
-        <v>1329</v>
+        <v>2228</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>740</v>
+        <v>579</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>4</v>
@@ -40078,10 +40078,10 @@
     </row>
     <row r="95" spans="1:4" ht="15.01" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>973</v>
+        <v>2238</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>740</v>
+        <v>579</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>4</v>
@@ -40092,10 +40092,10 @@
     </row>
     <row r="96" spans="1:4" ht="15.01" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>973</v>
+        <v>2110</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>295</v>
+        <v>579</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>4</v>
@@ -40106,10 +40106,10 @@
     </row>
     <row r="97" spans="1:4" ht="15.01" customHeight="1">
       <c r="A97" s="3" t="s">
-        <v>2650</v>
+        <v>1436</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>295</v>
+        <v>649</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>4</v>
@@ -40120,10 +40120,10 @@
     </row>
     <row r="98" spans="1:4" ht="15.01" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>2650</v>
+        <v>1404</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>280</v>
+        <v>649</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>4</v>
@@ -40134,10 +40134,10 @@
     </row>
     <row r="99" spans="1:4" ht="15.01" customHeight="1">
       <c r="A99" s="3" t="s">
-        <v>2650</v>
+        <v>1404</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>4</v>
@@ -40148,10 +40148,10 @@
     </row>
     <row r="100" spans="1:4" ht="15.01" customHeight="1">
       <c r="A100" s="3" t="s">
-        <v>2650</v>
+        <v>2110</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>326</v>
+        <v>262</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>4</v>
@@ -40162,10 +40162,10 @@
     </row>
     <row r="101" spans="1:4" ht="15.01" customHeight="1">
       <c r="A101" s="3" t="s">
-        <v>2650</v>
+        <v>2641</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>608</v>
+        <v>262</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>4</v>
@@ -40176,10 +40176,10 @@
     </row>
     <row r="102" spans="1:4" ht="15.01" customHeight="1">
       <c r="A102" s="3" t="s">
-        <v>2650</v>
+        <v>2641</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>646</v>
+        <v>357</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>4</v>
@@ -40190,10 +40190,10 @@
     </row>
     <row r="103" spans="1:4" ht="15.01" customHeight="1">
       <c r="A103" s="3" t="s">
-        <v>2650</v>
+        <v>2631</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>570</v>
+        <v>357</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>4</v>
@@ -40204,10 +40204,10 @@
     </row>
     <row r="104" spans="1:4" ht="15.01" customHeight="1">
       <c r="A104" s="3" t="s">
-        <v>2650</v>
+        <v>2631</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>306</v>
+        <v>812</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>4</v>
@@ -40218,10 +40218,10 @@
     </row>
     <row r="105" spans="1:4" ht="15.01" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>2914</v>
+        <v>1404</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>295</v>
+        <v>812</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>4</v>
@@ -40232,10 +40232,10 @@
     </row>
     <row r="106" spans="1:4" ht="15.01" customHeight="1">
       <c r="A106" s="3" t="s">
-        <v>2914</v>
+        <v>2304</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>594</v>
+        <v>812</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>4</v>
@@ -40246,10 +40246,10 @@
     </row>
     <row r="107" spans="1:4" ht="15.01" customHeight="1">
       <c r="A107" s="3" t="s">
-        <v>2914</v>
+        <v>2304</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>740</v>
+        <v>562</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>4</v>
@@ -40260,10 +40260,10 @@
     </row>
     <row r="108" spans="1:4" ht="15.01" customHeight="1">
       <c r="A108" s="3" t="s">
-        <v>2914</v>
+        <v>2506</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>280</v>
+        <v>562</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>4</v>
@@ -40274,10 +40274,10 @@
     </row>
     <row r="109" spans="1:4" ht="15.01" customHeight="1">
       <c r="A109" s="3" t="s">
-        <v>2914</v>
+        <v>1319</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>326</v>
+        <v>562</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>4</v>
@@ -40288,10 +40288,10 @@
     </row>
     <row r="110" spans="1:4" ht="15.01" customHeight="1">
       <c r="A110" s="3" t="s">
-        <v>2816</v>
+        <v>2631</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>295</v>
+        <v>594</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>4</v>
@@ -40302,10 +40302,10 @@
     </row>
     <row r="111" spans="1:4" ht="15.01" customHeight="1">
       <c r="A111" s="3" t="s">
-        <v>2269</v>
+        <v>2631</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>4</v>
@@ -40316,10 +40316,10 @@
     </row>
     <row r="112" spans="1:4" ht="15.01" customHeight="1">
       <c r="A112" s="3" t="s">
-        <v>2269</v>
+        <v>2631</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>4</v>
@@ -40330,52 +40330,52 @@
     </row>
     <row r="113" spans="1:4" ht="15.01" customHeight="1">
       <c r="A113" s="3" t="s">
-        <v>2641</v>
+        <v>1907</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>262</v>
+        <v>357</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.01" customHeight="1">
       <c r="A114" s="3" t="s">
-        <v>2641</v>
+        <v>1907</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.01" customHeight="1">
       <c r="A115" s="3" t="s">
-        <v>1404</v>
+        <v>1907</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>649</v>
+        <v>401</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.01" customHeight="1">
       <c r="A116" s="3" t="s">
-        <v>1404</v>
+        <v>2626</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>354</v>
+        <v>401</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>4</v>
@@ -40386,10 +40386,10 @@
     </row>
     <row r="117" spans="1:4" ht="15.01" customHeight="1">
       <c r="A117" s="3" t="s">
-        <v>1404</v>
+        <v>2626</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>357</v>
+        <v>422</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>4</v>
@@ -40400,10 +40400,10 @@
     </row>
     <row r="118" spans="1:4" ht="15.01" customHeight="1">
       <c r="A118" s="3" t="s">
-        <v>1939</v>
+        <v>2040</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>357</v>
+        <v>422</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>4</v>
@@ -40414,10 +40414,10 @@
     </row>
     <row r="119" spans="1:4" ht="15.01" customHeight="1">
       <c r="A119" s="3" t="s">
-        <v>2617</v>
+        <v>2040</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>357</v>
+        <v>646</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>4</v>
@@ -40428,10 +40428,10 @@
     </row>
     <row r="120" spans="1:4" ht="15.01" customHeight="1">
       <c r="A120" s="3" t="s">
-        <v>2641</v>
+        <v>2040</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>357</v>
+        <v>666</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>4</v>
@@ -40442,24 +40442,24 @@
     </row>
     <row r="121" spans="1:4" ht="15.01" customHeight="1">
       <c r="A121" s="3" t="s">
-        <v>1907</v>
+        <v>2092</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>357</v>
+        <v>666</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>3082</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.01" customHeight="1">
       <c r="A122" s="3" t="s">
-        <v>1907</v>
+        <v>1930</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>401</v>
+        <v>666</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>4</v>
@@ -40470,24 +40470,24 @@
     </row>
     <row r="123" spans="1:4" ht="15.01" customHeight="1">
       <c r="A123" s="3" t="s">
-        <v>2626</v>
+        <v>1930</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>401</v>
+        <v>326</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.01" customHeight="1">
       <c r="A124" s="3" t="s">
-        <v>2626</v>
+        <v>1930</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>326</v>
+        <v>608</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>4</v>
@@ -40498,10 +40498,10 @@
     </row>
     <row r="125" spans="1:4" ht="15.01" customHeight="1">
       <c r="A125" s="3" t="s">
-        <v>2626</v>
+        <v>2110</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>413</v>
+        <v>608</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>4</v>
@@ -40512,10 +40512,10 @@
     </row>
     <row r="126" spans="1:4" ht="15.01" customHeight="1">
       <c r="A126" s="3" t="s">
-        <v>2626</v>
+        <v>2451</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>439</v>
+        <v>608</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>4</v>
@@ -40526,10 +40526,10 @@
     </row>
     <row r="127" spans="1:4" ht="15.01" customHeight="1">
       <c r="A127" s="3" t="s">
-        <v>1653</v>
+        <v>2451</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>439</v>
+        <v>740</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>4</v>
@@ -40540,10 +40540,10 @@
     </row>
     <row r="128" spans="1:4" ht="15.01" customHeight="1">
       <c r="A128" s="3" t="s">
-        <v>1653</v>
+        <v>2110</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>194</v>
+        <v>740</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>4</v>
@@ -40554,24 +40554,24 @@
     </row>
     <row r="129" spans="1:4" ht="15.01" customHeight="1">
       <c r="A129" s="3" t="s">
-        <v>2563</v>
+        <v>2617</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>194</v>
+        <v>740</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.01" customHeight="1">
       <c r="A130" s="3" t="s">
-        <v>2563</v>
+        <v>1319</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>646</v>
+        <v>740</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>4</v>
@@ -40582,10 +40582,10 @@
     </row>
     <row r="131" spans="1:4" ht="15.01" customHeight="1">
       <c r="A131" s="3" t="s">
-        <v>2626</v>
+        <v>2269</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>646</v>
+        <v>740</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>4</v>
@@ -40596,10 +40596,10 @@
     </row>
     <row r="132" spans="1:4" ht="15.01" customHeight="1">
       <c r="A132" s="3" t="s">
-        <v>2626</v>
+        <v>2269</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>594</v>
+        <v>646</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>4</v>
@@ -40610,52 +40610,52 @@
     </row>
     <row r="133" spans="1:4" ht="15.01" customHeight="1">
       <c r="A133" s="3" t="s">
-        <v>2626</v>
+        <v>2269</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>422</v>
+        <v>548</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.01" customHeight="1">
       <c r="A134" s="3" t="s">
-        <v>2617</v>
+        <v>2269</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>422</v>
+        <v>167</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.01" customHeight="1">
       <c r="A135" s="3" t="s">
-        <v>1916</v>
+        <v>2571</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>422</v>
+        <v>167</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.01" customHeight="1">
       <c r="A136" s="3" t="s">
-        <v>2152</v>
+        <v>2571</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>422</v>
+        <v>326</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>4</v>
@@ -40666,10 +40666,10 @@
     </row>
     <row r="137" spans="1:4" ht="15.01" customHeight="1">
       <c r="A137" s="3" t="s">
-        <v>2152</v>
+        <v>2269</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>597</v>
+        <v>262</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>4</v>
@@ -40680,10 +40680,10 @@
     </row>
     <row r="138" spans="1:4" ht="15.01" customHeight="1">
       <c r="A138" s="3" t="s">
-        <v>2152</v>
+        <v>2269</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>4</v>
@@ -40694,10 +40694,10 @@
     </row>
     <row r="139" spans="1:4" ht="15.01" customHeight="1">
       <c r="A139" s="3" t="s">
-        <v>2152</v>
+        <v>2816</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>365</v>
+        <v>295</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>4</v>
@@ -40708,24 +40708,24 @@
     </row>
     <row r="140" spans="1:4" ht="15.01" customHeight="1">
       <c r="A140" s="3" t="s">
-        <v>2152</v>
+        <v>2914</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>712</v>
+        <v>295</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.01" customHeight="1">
       <c r="A141" s="3" t="s">
-        <v>2040</v>
+        <v>2914</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>422</v>
+        <v>326</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>4</v>
@@ -40736,10 +40736,10 @@
     </row>
     <row r="142" spans="1:4" ht="15.01" customHeight="1">
       <c r="A142" s="3" t="s">
-        <v>2040</v>
+        <v>2914</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>4</v>
@@ -40750,10 +40750,10 @@
     </row>
     <row r="143" spans="1:4" ht="15.01" customHeight="1">
       <c r="A143" s="3" t="s">
-        <v>2040</v>
+        <v>2914</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>280</v>
+        <v>740</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>4</v>
@@ -40764,10 +40764,10 @@
     </row>
     <row r="144" spans="1:4" ht="15.01" customHeight="1">
       <c r="A144" s="3" t="s">
-        <v>2040</v>
+        <v>2914</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>666</v>
+        <v>594</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>4</v>
@@ -40778,38 +40778,38 @@
     </row>
     <row r="145" spans="1:4" ht="15.01" customHeight="1">
       <c r="A145" s="3" t="s">
-        <v>1930</v>
+        <v>2650</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>666</v>
+        <v>295</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.01" customHeight="1">
       <c r="A146" s="3" t="s">
-        <v>2092</v>
+        <v>2650</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>666</v>
+        <v>306</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.01" customHeight="1">
       <c r="A147" s="3" t="s">
-        <v>2040</v>
+        <v>2650</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>646</v>
+        <v>570</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>4</v>
@@ -40820,7 +40820,7 @@
     </row>
     <row r="148" spans="1:4" ht="15.01" customHeight="1">
       <c r="A148" s="3" t="s">
-        <v>1907</v>
+        <v>2650</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>646</v>
@@ -40829,15 +40829,15 @@
         <v>4</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.01" customHeight="1">
       <c r="A149" s="3" t="s">
-        <v>2631</v>
+        <v>2650</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>357</v>
+        <v>608</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>4</v>
@@ -40848,10 +40848,10 @@
     </row>
     <row r="150" spans="1:4" ht="15.01" customHeight="1">
       <c r="A150" s="3" t="s">
-        <v>2631</v>
+        <v>2650</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>229</v>
+        <v>326</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>4</v>
@@ -40862,10 +40862,10 @@
     </row>
     <row r="151" spans="1:4" ht="15.01" customHeight="1">
       <c r="A151" s="3" t="s">
-        <v>2631</v>
+        <v>2650</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>4</v>
@@ -40876,10 +40876,10 @@
     </row>
     <row r="152" spans="1:4" ht="15.01" customHeight="1">
       <c r="A152" s="3" t="s">
-        <v>2631</v>
+        <v>2650</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>594</v>
+        <v>280</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>4</v>
@@ -40890,10 +40890,10 @@
     </row>
     <row r="153" spans="1:4" ht="15.01" customHeight="1">
       <c r="A153" s="3" t="s">
-        <v>2631</v>
+        <v>973</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>812</v>
+        <v>295</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>4</v>
@@ -40904,10 +40904,10 @@
     </row>
     <row r="154" spans="1:4" ht="15.01" customHeight="1">
       <c r="A154" s="3" t="s">
-        <v>2304</v>
+        <v>973</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>812</v>
+        <v>740</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>4</v>
@@ -40918,10 +40918,10 @@
     </row>
     <row r="155" spans="1:4" ht="15.01" customHeight="1">
       <c r="A155" s="3" t="s">
-        <v>2304</v>
+        <v>1329</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>562</v>
+        <v>740</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>4</v>
@@ -40932,10 +40932,10 @@
     </row>
     <row r="156" spans="1:4" ht="15.01" customHeight="1">
       <c r="A156" s="3" t="s">
-        <v>1319</v>
+        <v>1329</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>562</v>
+        <v>321</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>4</v>
@@ -40946,10 +40946,10 @@
     </row>
     <row r="157" spans="1:4" ht="15.01" customHeight="1">
       <c r="A157" s="3" t="s">
-        <v>2506</v>
+        <v>2617</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>562</v>
+        <v>321</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>4</v>
@@ -40960,10 +40960,10 @@
     </row>
     <row r="158" spans="1:4" ht="15.01" customHeight="1">
       <c r="A158" s="3" t="s">
-        <v>1404</v>
+        <v>2110</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>812</v>
+        <v>321</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>4</v>
@@ -40974,10 +40974,10 @@
     </row>
     <row r="159" spans="1:4" ht="15.01" customHeight="1">
       <c r="A159" s="3" t="s">
-        <v>1404</v>
+        <v>1289</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>262</v>
+        <v>321</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>4</v>
@@ -40988,10 +40988,10 @@
     </row>
     <row r="160" spans="1:4" ht="15.01" customHeight="1">
       <c r="A160" s="3" t="s">
-        <v>1436</v>
+        <v>1289</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>649</v>
+        <v>318</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>4</v>
@@ -41002,10 +41002,10 @@
     </row>
     <row r="161" spans="1:4" ht="15.01" customHeight="1">
       <c r="A161" s="3" t="s">
-        <v>1436</v>
+        <v>2506</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>579</v>
+        <v>318</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>4</v>
@@ -41019,7 +41019,7 @@
         <v>2110</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>579</v>
+        <v>318</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>4</v>
@@ -41030,10 +41030,10 @@
     </row>
     <row r="163" spans="1:4" ht="15.01" customHeight="1">
       <c r="A163" s="3" t="s">
-        <v>2238</v>
+        <v>1298</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>579</v>
+        <v>318</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>4</v>
@@ -41044,10 +41044,10 @@
     </row>
     <row r="164" spans="1:4" ht="15.01" customHeight="1">
       <c r="A164" s="3" t="s">
-        <v>2228</v>
+        <v>1298</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>579</v>
+        <v>461</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>4</v>
@@ -41058,24 +41058,24 @@
     </row>
     <row r="165" spans="1:4" ht="15.01" customHeight="1">
       <c r="A165" s="3" t="s">
-        <v>1436</v>
+        <v>2451</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.01" customHeight="1">
       <c r="A166" s="3" t="s">
-        <v>1436</v>
+        <v>1305</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>803</v>
+        <v>321</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>4</v>
@@ -41086,10 +41086,10 @@
     </row>
     <row r="167" spans="1:4" ht="15.01" customHeight="1">
       <c r="A167" s="3" t="s">
-        <v>1237</v>
+        <v>1305</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>803</v>
+        <v>603</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>4</v>
@@ -41100,24 +41100,24 @@
     </row>
     <row r="168" spans="1:4" ht="15.01" customHeight="1">
       <c r="A168" s="3" t="s">
-        <v>1245</v>
+        <v>2473</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>803</v>
+        <v>603</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.01" customHeight="1">
       <c r="A169" s="3" t="s">
-        <v>2055</v>
+        <v>1305</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>803</v>
+        <v>306</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>4</v>
@@ -41128,10 +41128,10 @@
     </row>
     <row r="170" spans="1:4" ht="15.01" customHeight="1">
       <c r="A170" s="3" t="s">
-        <v>2055</v>
+        <v>1329</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>652</v>
+        <v>570</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>4</v>
@@ -41142,10 +41142,10 @@
     </row>
     <row r="171" spans="1:4" ht="15.01" customHeight="1">
       <c r="A171" s="3" t="s">
-        <v>2055</v>
+        <v>1329</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>720</v>
+        <v>691</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>4</v>
@@ -41156,10 +41156,10 @@
     </row>
     <row r="172" spans="1:4" ht="15.01" customHeight="1">
       <c r="A172" s="3" t="s">
-        <v>2055</v>
+        <v>2228</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>306</v>
+        <v>691</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>4</v>
@@ -41170,10 +41170,10 @@
     </row>
     <row r="173" spans="1:4" ht="15.01" customHeight="1">
       <c r="A173" s="3" t="s">
-        <v>2055</v>
+        <v>1530</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>476</v>
+        <v>740</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>4</v>
@@ -41184,10 +41184,10 @@
     </row>
     <row r="174" spans="1:4" ht="15.01" customHeight="1">
       <c r="A174" s="3" t="s">
-        <v>2110</v>
+        <v>1149</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>262</v>
+        <v>740</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>4</v>
@@ -41198,10 +41198,10 @@
     </row>
     <row r="175" spans="1:4" ht="15.01" customHeight="1">
       <c r="A175" s="3" t="s">
-        <v>2269</v>
+        <v>1149</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>167</v>
+        <v>434</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>4</v>
@@ -41212,52 +41212,52 @@
     </row>
     <row r="176" spans="1:4" ht="15.01" customHeight="1">
       <c r="A176" s="3" t="s">
-        <v>2571</v>
+        <v>2617</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>167</v>
+        <v>434</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.01" customHeight="1">
       <c r="A177" s="3" t="s">
-        <v>2571</v>
+        <v>2451</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.01" customHeight="1">
       <c r="A178" s="3" t="s">
-        <v>2269</v>
+        <v>2451</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>548</v>
+        <v>247</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.01" customHeight="1">
       <c r="A179" s="3" t="s">
-        <v>2269</v>
+        <v>2451</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>740</v>
+        <v>326</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>4</v>
@@ -41268,10 +41268,10 @@
     </row>
     <row r="180" spans="1:4" ht="15.01" customHeight="1">
       <c r="A180" s="3" t="s">
-        <v>2269</v>
+        <v>2259</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>646</v>
+        <v>608</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>4</v>
@@ -41282,10 +41282,10 @@
     </row>
     <row r="181" spans="1:4" ht="15.01" customHeight="1">
       <c r="A181" s="3" t="s">
-        <v>1319</v>
+        <v>2259</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>740</v>
+        <v>473</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>4</v>
@@ -41296,24 +41296,24 @@
     </row>
     <row r="182" spans="1:4" ht="15.01" customHeight="1">
       <c r="A182" s="3" t="s">
-        <v>2617</v>
+        <v>2259</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>740</v>
+        <v>646</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.01" customHeight="1">
       <c r="A183" s="3" t="s">
-        <v>2110</v>
+        <v>2040</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>740</v>
+        <v>280</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>4</v>
@@ -41324,10 +41324,10 @@
     </row>
     <row r="184" spans="1:4" ht="15.01" customHeight="1">
       <c r="A184" s="3" t="s">
-        <v>2451</v>
+        <v>2040</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>740</v>
+        <v>306</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>4</v>
@@ -41338,24 +41338,24 @@
     </row>
     <row r="185" spans="1:4" ht="15.01" customHeight="1">
       <c r="A185" s="3" t="s">
-        <v>2617</v>
+        <v>2152</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>570</v>
+        <v>422</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15.01" customHeight="1">
       <c r="A186" s="3" t="s">
-        <v>2617</v>
+        <v>2152</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>247</v>
+        <v>712</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>4</v>
@@ -41366,10 +41366,10 @@
     </row>
     <row r="187" spans="1:4" ht="15.01" customHeight="1">
       <c r="A187" s="3" t="s">
-        <v>1329</v>
+        <v>2152</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>321</v>
+        <v>365</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>4</v>
@@ -41380,38 +41380,38 @@
     </row>
     <row r="188" spans="1:4" ht="15.01" customHeight="1">
       <c r="A188" s="3" t="s">
-        <v>1926</v>
+        <v>2152</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.01" customHeight="1">
       <c r="A189" s="3" t="s">
-        <v>1926</v>
+        <v>2152</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>280</v>
+        <v>597</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.01" customHeight="1">
       <c r="A190" s="3" t="s">
-        <v>1926</v>
+        <v>1916</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>658</v>
+        <v>422</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>4</v>
@@ -41422,24 +41422,24 @@
     </row>
     <row r="191" spans="1:4" ht="15.01" customHeight="1">
       <c r="A191" s="3" t="s">
-        <v>931</v>
+        <v>2617</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>658</v>
+        <v>422</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>3082</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.01" customHeight="1">
       <c r="A192" s="3" t="s">
-        <v>931</v>
+        <v>2626</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>247</v>
+        <v>594</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>4</v>
@@ -41450,24 +41450,24 @@
     </row>
     <row r="193" spans="1:4" ht="15.01" customHeight="1">
       <c r="A193" s="3" t="s">
-        <v>2092</v>
+        <v>2626</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>658</v>
+        <v>646</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.01" customHeight="1">
       <c r="A194" s="3" t="s">
-        <v>2282</v>
+        <v>2626</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>658</v>
+        <v>439</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>4</v>
@@ -41478,10 +41478,10 @@
     </row>
     <row r="195" spans="1:4" ht="15.01" customHeight="1">
       <c r="A195" s="3" t="s">
-        <v>1087</v>
+        <v>1653</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>658</v>
+        <v>439</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>4</v>
@@ -41492,10 +41492,10 @@
     </row>
     <row r="196" spans="1:4" ht="15.01" customHeight="1">
       <c r="A196" s="3" t="s">
-        <v>1087</v>
+        <v>1653</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>4</v>
@@ -41506,24 +41506,24 @@
     </row>
     <row r="197" spans="1:4" ht="15.01" customHeight="1">
       <c r="A197" s="3" t="s">
-        <v>1087</v>
+        <v>2563</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>487</v>
+        <v>194</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.01" customHeight="1">
       <c r="A198" s="3" t="s">
-        <v>1087</v>
+        <v>2563</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>4</v>
@@ -41534,10 +41534,10 @@
     </row>
     <row r="199" spans="1:4" ht="15.01" customHeight="1">
       <c r="A199" s="3" t="s">
-        <v>1916</v>
+        <v>2626</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>658</v>
+        <v>413</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>4</v>
@@ -41548,10 +41548,10 @@
     </row>
     <row r="200" spans="1:4" ht="15.01" customHeight="1">
       <c r="A200" s="3" t="s">
-        <v>2672</v>
+        <v>2626</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>658</v>
+        <v>326</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>4</v>
@@ -41562,10 +41562,10 @@
     </row>
     <row r="201" spans="1:4" ht="15.01" customHeight="1">
       <c r="A201" s="3" t="s">
-        <v>2672</v>
+        <v>2617</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>326</v>
+        <v>357</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>4</v>
@@ -41576,10 +41576,10 @@
     </row>
     <row r="202" spans="1:4" ht="15.01" customHeight="1">
       <c r="A202" s="3" t="s">
-        <v>2923</v>
+        <v>1939</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>658</v>
+        <v>357</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>4</v>
@@ -41590,10 +41590,10 @@
     </row>
     <row r="203" spans="1:4" ht="15.01" customHeight="1">
       <c r="A203" s="3" t="s">
-        <v>2506</v>
+        <v>1404</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>658</v>
+        <v>357</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>4</v>
@@ -41604,24 +41604,24 @@
     </row>
     <row r="204" spans="1:4" ht="15.01" customHeight="1">
       <c r="A204" s="3" t="s">
-        <v>1926</v>
+        <v>2641</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.01" customHeight="1">
       <c r="A205" s="3" t="s">
-        <v>992</v>
+        <v>1404</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>4</v>
@@ -41632,38 +41632,38 @@
     </row>
     <row r="206" spans="1:4" ht="15.01" customHeight="1">
       <c r="A206" s="3" t="s">
-        <v>992</v>
+        <v>2839</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>591</v>
+        <v>301</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.01" customHeight="1">
       <c r="A207" s="3" t="s">
-        <v>2092</v>
+        <v>2839</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>591</v>
+        <v>368</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.01" customHeight="1">
       <c r="A208" s="3" t="s">
-        <v>2959</v>
+        <v>2839</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>591</v>
+        <v>527</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>4</v>
@@ -41674,10 +41674,10 @@
     </row>
     <row r="209" spans="1:4" ht="15.01" customHeight="1">
       <c r="A209" s="3" t="s">
-        <v>2959</v>
+        <v>2210</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>280</v>
+        <v>527</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>4</v>
@@ -41688,10 +41688,10 @@
     </row>
     <row r="210" spans="1:4" ht="15.01" customHeight="1">
       <c r="A210" s="3" t="s">
-        <v>2959</v>
+        <v>2110</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>326</v>
+        <v>527</v>
       </c>
       <c r="C210" s="3" t="s">
         <v>4</v>
@@ -41702,10 +41702,10 @@
     </row>
     <row r="211" spans="1:4" ht="15.01" customHeight="1">
       <c r="A211" s="3" t="s">
-        <v>2959</v>
+        <v>1373</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>697</v>
+        <v>527</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>4</v>
@@ -41716,10 +41716,10 @@
     </row>
     <row r="212" spans="1:4" ht="15.01" customHeight="1">
       <c r="A212" s="3" t="s">
-        <v>2110</v>
+        <v>1373</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>697</v>
+        <v>306</v>
       </c>
       <c r="C212" s="3" t="s">
         <v>4</v>
@@ -41730,10 +41730,10 @@
     </row>
     <row r="213" spans="1:4" ht="15.01" customHeight="1">
       <c r="A213" s="3" t="s">
-        <v>2717</v>
+        <v>1373</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>697</v>
+        <v>326</v>
       </c>
       <c r="C213" s="3" t="s">
         <v>4</v>
@@ -41744,10 +41744,10 @@
     </row>
     <row r="214" spans="1:4" ht="15.01" customHeight="1">
       <c r="A214" s="3" t="s">
-        <v>2717</v>
+        <v>2506</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>559</v>
+        <v>301</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>4</v>
@@ -41758,10 +41758,10 @@
     </row>
     <row r="215" spans="1:4" ht="15.01" customHeight="1">
       <c r="A215" s="3" t="s">
-        <v>2015</v>
+        <v>2110</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>559</v>
+        <v>301</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>4</v>
@@ -41772,24 +41772,24 @@
     </row>
     <row r="216" spans="1:4" ht="15.01" customHeight="1">
       <c r="A216" s="3" t="s">
-        <v>2015</v>
+        <v>2825</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>720</v>
+        <v>301</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15.01" customHeight="1">
       <c r="A217" s="3" t="s">
-        <v>2731</v>
+        <v>2825</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>697</v>
+        <v>365</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>4</v>
@@ -41800,10 +41800,10 @@
     </row>
     <row r="218" spans="1:4" ht="15.01" customHeight="1">
       <c r="A218" s="3" t="s">
-        <v>2731</v>
+        <v>2825</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>172</v>
+        <v>720</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>4</v>
@@ -41814,10 +41814,10 @@
     </row>
     <row r="219" spans="1:4" ht="15.01" customHeight="1">
       <c r="A219" s="3" t="s">
-        <v>2731</v>
+        <v>2825</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>646</v>
+        <v>368</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>4</v>
@@ -41828,49 +41828,49 @@
     </row>
     <row r="220" spans="1:4" ht="15.01" customHeight="1">
       <c r="A220" s="3" t="s">
-        <v>2754</v>
+        <v>2825</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>697</v>
+        <v>326</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15.01" customHeight="1">
       <c r="A221" s="3" t="s">
-        <v>2754</v>
+        <v>2825</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>326</v>
+        <v>476</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.01" customHeight="1">
       <c r="A222" s="3" t="s">
-        <v>2754</v>
+        <v>2554</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>280</v>
+        <v>720</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15.01" customHeight="1">
       <c r="A223" s="3" t="s">
-        <v>2754</v>
+        <v>2554</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>594</v>
@@ -41879,32 +41879,32 @@
         <v>4</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15.01" customHeight="1">
       <c r="A224" s="3" t="s">
-        <v>2754</v>
+        <v>2110</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>600</v>
+        <v>476</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15.01" customHeight="1">
       <c r="A225" s="3" t="s">
-        <v>1967</v>
+        <v>2506</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>600</v>
+        <v>476</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>3080</v>
@@ -41912,24 +41912,24 @@
     </row>
     <row r="226" spans="1:4" ht="15.01" customHeight="1">
       <c r="A226" s="3" t="s">
-        <v>1976</v>
+        <v>2055</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>600</v>
+        <v>720</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15.01" customHeight="1">
       <c r="A227" s="3" t="s">
-        <v>1976</v>
+        <v>2055</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>594</v>
+        <v>652</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>4</v>
@@ -41940,27 +41940,27 @@
     </row>
     <row r="228" spans="1:4" ht="15.01" customHeight="1">
       <c r="A228" s="3" t="s">
-        <v>2092</v>
+        <v>2110</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>600</v>
+        <v>306</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15.01" customHeight="1">
       <c r="A229" s="3" t="s">
-        <v>2110</v>
+        <v>2101</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>600</v>
+        <v>306</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>3080</v>
@@ -41968,10 +41968,10 @@
     </row>
     <row r="230" spans="1:4" ht="15.01" customHeight="1">
       <c r="A230" s="3" t="s">
-        <v>1967</v>
+        <v>2101</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>363</v>
+        <v>280</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>4</v>
@@ -41982,38 +41982,38 @@
     </row>
     <row r="231" spans="1:4" ht="15.01" customHeight="1">
       <c r="A231" s="3" t="s">
-        <v>1967</v>
+        <v>2092</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>597</v>
+        <v>306</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15.01" customHeight="1">
       <c r="A232" s="3" t="s">
-        <v>2754</v>
+        <v>2084</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>646</v>
+        <v>306</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>3082</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15.01" customHeight="1">
       <c r="A233" s="3" t="s">
-        <v>2790</v>
+        <v>2084</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>4</v>
@@ -42024,7 +42024,7 @@
     </row>
     <row r="234" spans="1:4" ht="15.01" customHeight="1">
       <c r="A234" s="3" t="s">
-        <v>1916</v>
+        <v>1129</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>306</v>
@@ -42033,43 +42033,43 @@
         <v>4</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15.01" customHeight="1">
       <c r="A235" s="3" t="s">
-        <v>2110</v>
+        <v>1916</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>527</v>
+        <v>646</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.01" customHeight="1">
       <c r="A236" s="3" t="s">
-        <v>2210</v>
+        <v>1916</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>527</v>
+        <v>280</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.01" customHeight="1">
       <c r="A237" s="3" t="s">
-        <v>2839</v>
+        <v>1087</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>368</v>
+        <v>658</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>4</v>
@@ -42080,10 +42080,10 @@
     </row>
     <row r="238" spans="1:4" ht="15.01" customHeight="1">
       <c r="A238" s="3" t="s">
-        <v>2825</v>
+        <v>1087</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>368</v>
+        <v>640</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>4</v>
@@ -42094,10 +42094,10 @@
     </row>
     <row r="239" spans="1:4" ht="15.01" customHeight="1">
       <c r="A239" s="3" t="s">
-        <v>2219</v>
+        <v>2506</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>368</v>
+        <v>640</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>4</v>
@@ -42108,10 +42108,10 @@
     </row>
     <row r="240" spans="1:4" ht="15.01" customHeight="1">
       <c r="A240" s="3" t="s">
-        <v>2228</v>
+        <v>1111</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>368</v>
+        <v>640</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>4</v>
@@ -42122,10 +42122,10 @@
     </row>
     <row r="241" spans="1:4" ht="15.01" customHeight="1">
       <c r="A241" s="3" t="s">
-        <v>1477</v>
+        <v>1159</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>368</v>
+        <v>640</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>4</v>
@@ -42136,10 +42136,10 @@
     </row>
     <row r="242" spans="1:4" ht="15.01" customHeight="1">
       <c r="A242" s="3" t="s">
-        <v>1477</v>
+        <v>1159</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>567</v>
+        <v>312</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>4</v>
@@ -42150,10 +42150,10 @@
     </row>
     <row r="243" spans="1:4" ht="15.01" customHeight="1">
       <c r="A243" s="3" t="s">
-        <v>1477</v>
+        <v>1019</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>470</v>
+        <v>312</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>4</v>
@@ -42164,10 +42164,10 @@
     </row>
     <row r="244" spans="1:4" ht="15.01" customHeight="1">
       <c r="A244" s="3" t="s">
-        <v>1319</v>
+        <v>1019</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>470</v>
+        <v>326</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>4</v>
@@ -42178,10 +42178,10 @@
     </row>
     <row r="245" spans="1:4" ht="15.01" customHeight="1">
       <c r="A245" s="3" t="s">
-        <v>2110</v>
+        <v>1028</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>470</v>
+        <v>312</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>4</v>
@@ -42192,10 +42192,10 @@
     </row>
     <row r="246" spans="1:4" ht="15.01" customHeight="1">
       <c r="A246" s="3" t="s">
-        <v>2699</v>
+        <v>1028</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>470</v>
+        <v>360</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>4</v>
@@ -42206,24 +42206,24 @@
     </row>
     <row r="247" spans="1:4" ht="15.01" customHeight="1">
       <c r="A247" s="3" t="s">
-        <v>2092</v>
+        <v>1028</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>470</v>
+        <v>259</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15.01" customHeight="1">
       <c r="A248" s="3" t="s">
-        <v>1282</v>
+        <v>1028</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>4</v>
@@ -42234,10 +42234,10 @@
     </row>
     <row r="249" spans="1:4" ht="15.01" customHeight="1">
       <c r="A249" s="3" t="s">
-        <v>2123</v>
+        <v>1087</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>368</v>
+        <v>487</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>4</v>
@@ -42248,10 +42248,10 @@
     </row>
     <row r="250" spans="1:4" ht="15.01" customHeight="1">
       <c r="A250" s="3" t="s">
-        <v>2123</v>
+        <v>1087</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>365</v>
+        <v>238</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>4</v>
@@ -42262,10 +42262,10 @@
     </row>
     <row r="251" spans="1:4" ht="15.01" customHeight="1">
       <c r="A251" s="3" t="s">
-        <v>2110</v>
+        <v>2282</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>368</v>
+        <v>658</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>4</v>
@@ -42276,10 +42276,10 @@
     </row>
     <row r="252" spans="1:4" ht="15.01" customHeight="1">
       <c r="A252" s="3" t="s">
-        <v>2587</v>
+        <v>2092</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>368</v>
+        <v>658</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>4</v>
@@ -42290,24 +42290,24 @@
     </row>
     <row r="253" spans="1:4" ht="15.01" customHeight="1">
       <c r="A253" s="3" t="s">
-        <v>2587</v>
+        <v>931</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>437</v>
+        <v>658</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>3080</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15.01" customHeight="1">
       <c r="A254" s="3" t="s">
-        <v>2587</v>
+        <v>931</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>365</v>
+        <v>247</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>4</v>
@@ -42318,10 +42318,10 @@
     </row>
     <row r="255" spans="1:4" ht="15.01" customHeight="1">
       <c r="A255" s="3" t="s">
-        <v>2587</v>
+        <v>2228</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>247</v>
+        <v>567</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>4</v>
@@ -42332,10 +42332,10 @@
     </row>
     <row r="256" spans="1:4" ht="15.01" customHeight="1">
       <c r="A256" s="3" t="s">
-        <v>2825</v>
+        <v>1319</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>720</v>
+        <v>567</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>4</v>
@@ -42346,10 +42346,10 @@
     </row>
     <row r="257" spans="1:4" ht="15.01" customHeight="1">
       <c r="A257" s="3" t="s">
-        <v>2825</v>
+        <v>2228</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>4</v>
@@ -42360,10 +42360,10 @@
     </row>
     <row r="258" spans="1:4" ht="15.01" customHeight="1">
       <c r="A258" s="3" t="s">
-        <v>2554</v>
+        <v>2219</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>476</v>
+        <v>536</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>4</v>
@@ -42374,10 +42374,10 @@
     </row>
     <row r="259" spans="1:4" ht="15.01" customHeight="1">
       <c r="A259" s="3" t="s">
-        <v>2506</v>
+        <v>2219</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>550</v>
+        <v>720</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>4</v>
@@ -42388,80 +42388,80 @@
     </row>
     <row r="260" spans="1:4" ht="15.01" customHeight="1">
       <c r="A260" s="3" t="s">
-        <v>2228</v>
+        <v>2754</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>550</v>
+        <v>326</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15.01" customHeight="1">
       <c r="A261" s="3" t="s">
-        <v>2506</v>
+        <v>2773</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>818</v>
+        <v>326</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15.01" customHeight="1">
       <c r="A262" s="3" t="s">
-        <v>2228</v>
+        <v>2773</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>818</v>
+        <v>743</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15.01" customHeight="1">
       <c r="A263" s="3" t="s">
-        <v>2506</v>
+        <v>2767</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>567</v>
+        <v>743</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15.01" customHeight="1">
       <c r="A264" s="3" t="s">
-        <v>2506</v>
+        <v>2767</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>720</v>
+        <v>326</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15.01" customHeight="1">
       <c r="A265" s="3" t="s">
-        <v>2335</v>
+        <v>2607</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>4</v>
@@ -42472,38 +42472,38 @@
     </row>
     <row r="266" spans="1:4" ht="15.01" customHeight="1">
       <c r="A266" s="3" t="s">
-        <v>2335</v>
+        <v>2378</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>594</v>
+        <v>326</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15.01" customHeight="1">
       <c r="A267" s="3" t="s">
-        <v>2335</v>
+        <v>2092</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>597</v>
+        <v>326</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15.01" customHeight="1">
       <c r="A268" s="3" t="s">
-        <v>2451</v>
+        <v>2959</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>608</v>
+        <v>280</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>4</v>
@@ -42514,13 +42514,13 @@
     </row>
     <row r="269" spans="1:4" ht="15.01" customHeight="1">
       <c r="A269" s="3" t="s">
-        <v>2219</v>
+        <v>2754</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>326</v>
+        <v>600</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D269" s="3" t="s">
         <v>3082</v>
@@ -42528,16 +42528,16 @@
     </row>
     <row r="270" spans="1:4" ht="15.01" customHeight="1">
       <c r="A270" s="3" t="s">
-        <v>2110</v>
+        <v>2754</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>326</v>
+        <v>594</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15.01" customHeight="1">
@@ -42545,7 +42545,7 @@
         <v>2110</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>608</v>
+        <v>280</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>4</v>
@@ -42556,16 +42556,16 @@
     </row>
     <row r="272" spans="1:4" ht="15.01" customHeight="1">
       <c r="A272" s="3" t="s">
-        <v>1916</v>
+        <v>2092</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>441</v>
+        <v>594</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>3080</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15.01" customHeight="1">
@@ -42573,24 +42573,24 @@
         <v>2092</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>280</v>
+        <v>597</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>3081</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15.01" customHeight="1">
       <c r="A274" s="3" t="s">
-        <v>2722</v>
+        <v>1967</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>280</v>
+        <v>600</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D274" s="3" t="s">
         <v>3080</v>
@@ -42598,10 +42598,10 @@
     </row>
     <row r="275" spans="1:4" ht="15.01" customHeight="1">
       <c r="A275" s="3" t="s">
-        <v>2722</v>
+        <v>1967</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>709</v>
+        <v>597</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>4</v>
@@ -42612,10 +42612,10 @@
     </row>
     <row r="276" spans="1:4" ht="15.01" customHeight="1">
       <c r="A276" s="3" t="s">
-        <v>2065</v>
+        <v>1967</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>4</v>
@@ -42626,10 +42626,10 @@
     </row>
     <row r="277" spans="1:4" ht="15.01" customHeight="1">
       <c r="A277" s="3" t="s">
-        <v>2065</v>
+        <v>2110</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>685</v>
+        <v>597</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>4</v>
@@ -42640,10 +42640,10 @@
     </row>
     <row r="278" spans="1:4" ht="15.01" customHeight="1">
       <c r="A278" s="3" t="s">
-        <v>2529</v>
+        <v>897</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>685</v>
+        <v>597</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>4</v>
@@ -42654,10 +42654,10 @@
     </row>
     <row r="279" spans="1:4" ht="15.01" customHeight="1">
       <c r="A279" s="3" t="s">
-        <v>2529</v>
+        <v>2430</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>594</v>
+        <v>365</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>4</v>
@@ -42668,10 +42668,10 @@
     </row>
     <row r="280" spans="1:4" ht="15.01" customHeight="1">
       <c r="A280" s="3" t="s">
-        <v>2529</v>
+        <v>2430</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>597</v>
+        <v>247</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>4</v>
@@ -42682,10 +42682,10 @@
     </row>
     <row r="281" spans="1:4" ht="15.01" customHeight="1">
       <c r="A281" s="3" t="s">
-        <v>2110</v>
+        <v>1078</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>536</v>
+        <v>365</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>4</v>
@@ -42696,10 +42696,10 @@
     </row>
     <row r="282" spans="1:4" ht="15.01" customHeight="1">
       <c r="A282" s="3" t="s">
-        <v>2110</v>
+        <v>1078</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>720</v>
+        <v>268</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>4</v>
@@ -42710,10 +42710,10 @@
     </row>
     <row r="283" spans="1:4" ht="15.01" customHeight="1">
       <c r="A283" s="3" t="s">
-        <v>1319</v>
+        <v>1559</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>570</v>
+        <v>268</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>4</v>
@@ -42724,10 +42724,10 @@
     </row>
     <row r="284" spans="1:4" ht="15.01" customHeight="1">
       <c r="A284" s="3" t="s">
-        <v>2228</v>
+        <v>1559</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>324</v>
+        <v>661</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>4</v>
@@ -42738,10 +42738,10 @@
     </row>
     <row r="285" spans="1:4" ht="15.01" customHeight="1">
       <c r="A285" s="3" t="s">
-        <v>2228</v>
+        <v>1567</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>507</v>
+        <v>661</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>4</v>
@@ -42752,10 +42752,10 @@
     </row>
     <row r="286" spans="1:4" ht="15.01" customHeight="1">
       <c r="A286" s="3" t="s">
-        <v>2228</v>
+        <v>1007</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>720</v>
+        <v>268</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>4</v>
@@ -42766,10 +42766,10 @@
     </row>
     <row r="287" spans="1:4" ht="15.01" customHeight="1">
       <c r="A287" s="3" t="s">
-        <v>2228</v>
+        <v>1078</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>792</v>
+        <v>247</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>4</v>
@@ -42780,10 +42780,10 @@
     </row>
     <row r="288" spans="1:4" ht="15.01" customHeight="1">
       <c r="A288" s="3" t="s">
-        <v>2219</v>
+        <v>2587</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>792</v>
+        <v>437</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>4</v>
@@ -42794,10 +42794,10 @@
     </row>
     <row r="289" spans="1:4" ht="15.01" customHeight="1">
       <c r="A289" s="3" t="s">
-        <v>2554</v>
+        <v>2110</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>792</v>
+        <v>570</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>4</v>
@@ -42811,7 +42811,7 @@
         <v>1319</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>792</v>
+        <v>536</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>4</v>
@@ -42822,10 +42822,10 @@
     </row>
     <row r="291" spans="1:4" ht="15.01" customHeight="1">
       <c r="A291" s="3" t="s">
-        <v>1259</v>
+        <v>2228</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>567</v>
+        <v>507</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>4</v>
@@ -42836,10 +42836,10 @@
     </row>
     <row r="292" spans="1:4" ht="15.01" customHeight="1">
       <c r="A292" s="3" t="s">
-        <v>1259</v>
+        <v>2228</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>286</v>
+        <v>324</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>4</v>
@@ -42850,10 +42850,10 @@
     </row>
     <row r="293" spans="1:4" ht="15.01" customHeight="1">
       <c r="A293" s="3" t="s">
-        <v>2554</v>
+        <v>2749</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>536</v>
+        <v>720</v>
       </c>
       <c r="C293" s="3" t="s">
         <v>4</v>
@@ -42864,10 +42864,10 @@
     </row>
     <row r="294" spans="1:4" ht="15.01" customHeight="1">
       <c r="A294" s="3" t="s">
-        <v>2219</v>
+        <v>2030</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>597</v>
+        <v>197</v>
       </c>
       <c r="C294" s="3" t="s">
         <v>4</v>

</xml_diff>